<commit_message>
solve cors issue,aad phases upload,modifications in some end points
</commit_message>
<xml_diff>
--- a/phasesproperties.xlsx
+++ b/phasesproperties.xlsx
@@ -278,385 +278,385 @@
     <t>OW/HV1-10A</t>
   </si>
   <si>
+    <t>Hillside</t>
+  </si>
+  <si>
+    <t>Townhouse</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>ff29216a-7dcf-eb11-8235-002248801d1c</t>
+  </si>
+  <si>
+    <t>HzrGqBLdYHM/oZ7X15eZiPqFzR5Fh3oi8td+Se1jaO12vTAouN9jZ28Zh09bWzJAu4/lVjMeTf2/vqzHcOHoSg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-10D</t>
+  </si>
+  <si>
+    <t>072a216a-7dcf-eb11-8235-002248801d1c</t>
+  </si>
+  <si>
+    <t>YGfaaeMV1tVrfsxOE1q5BtfnxhbEWasc/WhCB0M4w1jE3TLSk6P4XoXsWTdvUPDZizWJAPJRVyb2Kk0KfElrIw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-12D</t>
+  </si>
+  <si>
+    <t>d33523d3-b8bb-eb11-8236-000d3a2aa3e6</t>
+  </si>
+  <si>
+    <t>bwEfzxjV3QTZkAchrI95jB6O9Q72BNimF0Fr+E5Cc9YPQatQWBQgPRflN3HAESXvs1r2CiPlioljzp+e/+1ufA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-14D</t>
+  </si>
+  <si>
+    <t>a25fe136-c8df-eb11-bacb-000d3abc0501</t>
+  </si>
+  <si>
+    <t>nGIyZWpqlykKGjpR1DcwvtnIfK0fW2/z4NyVnLhp3UxTrO2Rhf1glw0u0mlyBjLw6QU7GjD3OU3ARm+zPsJ8ew==</t>
+  </si>
+  <si>
+    <t>OW/HV1-16D</t>
+  </si>
+  <si>
+    <t>410c4583-2b16-ec11-b6e5-6045bd8b892f</t>
+  </si>
+  <si>
+    <t>bC9gaTBL5N5KJ8ZDf3vkDzL+vKXwaEXqxp7MYoXQRH6U9vn7JctbIaYUlgRSbCeFYGqwvSor7UmmdzfKyQXMBw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-17D</t>
+  </si>
+  <si>
+    <t>be7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>tUEZ9xNVG+u3djAGBSsp5oQmW3kM7FYNydt7FHIaL/fVuAXKPKIG/tx/rdeu/oJIN7zQyfZaiDkO91XBn5SA+A==</t>
+  </si>
+  <si>
+    <t>OW/HV1-18A</t>
+  </si>
+  <si>
+    <t>c07a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>7Z8dgiurCfbwR44GB5glOl3Zx89nv95VQ5x+JLMZOgLEdp96ws14d1VdfPNEo0HOKpc9oEmaOHsPg/f/Ee1RgQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-18B</t>
+  </si>
+  <si>
+    <t>c37a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>6hEQvttsYYe+5tITldnplOe4jh79u1LNZ0fEE0sATIz2IHUpocgC87NaMf7jM4KeJlVtRcgdVFRdgA3wFxE3QA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-18C</t>
+  </si>
+  <si>
+    <t>c57a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>W+NwUuro+SZXPOOCdOEZyt7ewtrDh0YKm39vp4VBQlwqgiZ/D2DRot/TqKZ8+b1+bbHCeRzpezdu8CDpAuci/A==</t>
+  </si>
+  <si>
+    <t>OW/HV1-18D</t>
+  </si>
+  <si>
+    <t>Twinhouse</t>
+  </si>
+  <si>
+    <t>6b03c3e7-0a0b-ec11-b6e5-000d3aaf448c</t>
+  </si>
+  <si>
+    <t>HUMlmio1EdCu2Fam+88n/6wFcrEmcO4V93wgoaOr9XmNiCwdFK6iWnQOTpO72zqCWNTWoVxhTDJmZhV+esDMtQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-19B</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>6d03c3e7-0a0b-ec11-b6e5-000d3aaf448c</t>
+  </si>
+  <si>
+    <t>3HXGQ3uAF0SNZ+vUlFTEul4+ptEAuSsR97uC01asaIHLGWlltO3QSBHyhOl9EH5NSVa/Hb1Oq1RZz2hY++qesw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-19C</t>
+  </si>
+  <si>
+    <t>6f03c3e7-0a0b-ec11-b6e5-000d3aaf448c</t>
+  </si>
+  <si>
+    <t>KRqIUWg+i/oe7lrm1xtxd8NE8UitMGLgI+7Vp8BPt77PaPl0F8BboApuBbbrG+6WtxA+IUIDFY0+pP0J1tBxlw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-19D</t>
+  </si>
+  <si>
+    <t>af3523d3-b8bb-eb11-8236-000d3a2aa3e6</t>
+  </si>
+  <si>
+    <t>4Hb9fbTR9JWDiQXSUv6CqwuOUbZ94CsGQT+ITNS5IaKFhooydQZEIRvEeQljTTOqp39w5mldFml3rgTr4okdMA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-1TKB</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>c97a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>7h7rme1qC3TSq3CJ+ReITzjMMOjlY188bXhbHIb2qsu9Tby5f6ykSaz4l5QqOr0uRXkZGPyCZHNs0/OIXzuymw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-20B</t>
+  </si>
+  <si>
+    <t>d37a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>Y+DV810ZXTFsn7H1FxqgKrGTcPZq7fNehHC5OOoEhPmTrMnW5Ilkb9SmDwWuFJ78rYpri9jFICbvE+cE2zdZ8w==</t>
+  </si>
+  <si>
+    <t>OW/HV1-21B</t>
+  </si>
+  <si>
+    <t>d57a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>cbaxaqptmV9e6y3X4B2+DrB44rwQNm4ToL+3cPAB9UV3m0VYxjRMw4cnEvmya8XMqdlzQkPH1iqMpxUyh0nwaA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-21C</t>
+  </si>
+  <si>
+    <t>d77a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>qJqHCx7xzaB2Z3JL5T/lqHAd9W8aH5IvKzT77fQjScedQbLhvyep0yszsMuPimVEvfwDtsPOQ9xFYj84nOBs/w==</t>
+  </si>
+  <si>
+    <t>OW/HV1-21D</t>
+  </si>
+  <si>
+    <t>d97a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>T0xOk3D/cl/0qU4vkHDcGCI3P7owT6GacDrjrlys2fkxHwJR1ktcoxGEKRcqVCdNU8pTQGf54HdaKFhaqo2BXA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-21E</t>
+  </si>
+  <si>
+    <t>ac5fe136-c8df-eb11-bacb-000d3abc0501</t>
+  </si>
+  <si>
+    <t>ZxkPtn6oa9l/0e0uh+z785MlMF/mBZBnz5kZGy0hx4Uxo0BDCshbe8ETCCgPWIH8RaWWTWo2yQHqx7Wyi5ygzQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-22TA</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>de7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>u7IOD+iuQ5sKfDppYLR4h1wbCn7w39a9FYatrkIz5G0ycl41FmZYguHkAyBG+CZiIQRuSaMlI1bejHZfR586Kg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-23B</t>
+  </si>
+  <si>
+    <t>e67a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>cwLcmcvuhFJMO0kTvWeF5SRR0GS2CLSMt0fBLpHEm1WN8VCxpeWej93LjxIdiKnzPDToOUoGmNsFXCzWt0bPEg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-30A</t>
+  </si>
+  <si>
+    <t>eb7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>XiBjgAyX3/P3YUq+5RGRSq2/IcioNNcJfnt0o3/sI4AE9CD3ROYkQfYIiKFSg3l0EANhoYNtQO5XDMjgWe86xQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-30C</t>
+  </si>
+  <si>
+    <t>ef7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>3Waw/y+dN8e1Yq3QYProZOszj1m0XgV3LPZoxs8hanJftSN3/w89oUcsSNqMMjB/tlW/RyqpH94o2jbwn0bpuQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-30E</t>
+  </si>
+  <si>
+    <t>d7a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>SdBQ++rM0MSQlP9FOmMht2dIhTy2rP63P6Hdpz+aW9L0Bh1mt6L1V0QyNZ8b6d1wAef3eOM7mJM2uQ8owBNtWA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-33A</t>
+  </si>
+  <si>
+    <t>d9a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>kApVnIaMjaElQqwBEX5twXnTJeowq+zEt2ZK4CxG1gNSPpp/wgf63TzRxoFRf5UHeTLvmCCkQjRnl/dv99nG3A==</t>
+  </si>
+  <si>
+    <t>OW/HV1-33B</t>
+  </si>
+  <si>
+    <t>dba9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>x5799yTYqlsnPC52b2iyv0Mki0p0GlgSSkyFx+EMQpjuSNB9ct6YHKG3CiNFZqPW+K1dMOM7VYiHxwEEnJLk7g==</t>
+  </si>
+  <si>
+    <t>OW/HV1-33C</t>
+  </si>
+  <si>
+    <t>dda9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>lZnDQ1uD1O33c0I8nshrheSJmblZObhqe4EJkzVXRqgLHnHtCtu7ALRerV1+0O7oUTgsXFNMrRhhhKmZYOJnkw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-33D</t>
+  </si>
+  <si>
+    <t>dfa9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>8PTxyxB2ouNjbHGH1BWXy+bZWF3/jSoseypyt7QABgUVAmopls/cQadhhtVDobmHe/YWSVjs8HTEFdQE9YYOjA==</t>
+  </si>
+  <si>
+    <t>OW/HV1-34A</t>
+  </si>
+  <si>
+    <t>e1a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>hrrtixqGw4gTV9TZX1sdSSZSZazUtgh1b2UDhtBGciZbaaruqQnMoX4spe5SXNc6NRtk0M9K2vmgbLvGFKDXfg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-34B</t>
+  </si>
+  <si>
+    <t>e5a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
+  </si>
+  <si>
+    <t>LmT3c16H7xfuL+B7Wk/g0zXWnVCL9jrwks1+i3qy4draYOZbOr4h5bCnqV5xCHKFuSecL+D+Nebb3w4B7FRqcg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-34D</t>
+  </si>
+  <si>
+    <t>fd7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>GCIpDNkHqX4A8Hss2dfFWFwaiU5qEWfLVu2tNe0GKIHytoreXXqQHrrPuwwtd2YJ+yld3ngcskFASTYhfWbqnQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-35THA</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>ff7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>DGnwBSZQO5go6ZRsfoXHMKf/+FaHXiEO4ck7HSkVJXLUzMZVXzQmLAX+qTWJsPOuAFOY25GpQXrCSrH9ehc0YQ==</t>
+  </si>
+  <si>
+    <t>OW/HV1-35THB</t>
+  </si>
+  <si>
+    <t>017b50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>4yY1/rgt8ABrKOoCKUes8fuAgifZDmevoxiCQ7sU4/A+iagCY2reocH56he/OzPmW/yDyjV+eXGZuLtzGt/e8Q==</t>
+  </si>
+  <si>
+    <t>OW/HV1-36A</t>
+  </si>
+  <si>
+    <t>077b50c7-bb26-ec11-b6e5-000d3aa85461</t>
+  </si>
+  <si>
+    <t>yphCM63qZtgqwa6vy1eEhCnYyns6mIJf9WrSbItm1oqHlNwxJSdtqo3VMFGTsE1bE2dqr7USCyTd8iPgyJ+0eg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-36D</t>
+  </si>
+  <si>
+    <t>b838f9db-a6d1-eb11-8235-000d3abe8665</t>
+  </si>
+  <si>
+    <t>u5J4fE6/Z1oBcyUF3CauSQ+hQ61oOmEUz0N632nbvLa0y9j3XRobwH0btpBgOtGk9Lrzajk1Y1Jw3P4A7PQDZg==</t>
+  </si>
+  <si>
+    <t>OW/HV1-43-0-BL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>ba38f9db-a6d1-eb11-8235-000d3abe8665</t>
+  </si>
+  <si>
+    <t>Vy9uQEYloIRZT+8RFaPaZpdeCyZOgAEKYVEMT7lswXvlDbPWe9+t8dz8fgaEm4yra6sqV84D79ef5K+zYZHtAw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-43-1-BL</t>
+  </si>
+  <si>
+    <t>bc38f9db-a6d1-eb11-8235-000d3abe8665</t>
+  </si>
+  <si>
+    <t>fRj8ikVDxSej1ZM0tezdXeL2rQjs29i4w0Rtq96UFcszVmGoM1D25w/HgCz5UMKMcv+RXCojAld20QIQagJL/w==</t>
+  </si>
+  <si>
+    <t>OW/HV1-43-2-BL</t>
+  </si>
+  <si>
+    <t>c53523d3-b8bb-eb11-8236-000d3a2aa3e6</t>
+  </si>
+  <si>
+    <t>AsyjXTB1xOyTJ2yson9gtfJ9MiFKiITPdsf6eYCD+XLt6Bv3zsBaEDpNv4SwmfLFwV2pGP5s+ySISUwkd7G7hw==</t>
+  </si>
+  <si>
+    <t>OW/HV1-5D</t>
+  </si>
+  <si>
+    <t>2fbceaec-21be-eb11-8236-000d3a2aa437</t>
+  </si>
+  <si>
+    <t>zTXxXfGJg6U7Ue3ELjZcYSbhr3jdiU50OcJg7BOtmB+fH6N9qul0wMmtkeVjO5EP9kOScxk7fhgtjw25qTGs/g==</t>
+  </si>
+  <si>
+    <t>OW/HV1-8D</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hillside </t>
-  </si>
-  <si>
-    <t>Townhouse</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>ff29216a-7dcf-eb11-8235-002248801d1c</t>
-  </si>
-  <si>
-    <t>HzrGqBLdYHM/oZ7X15eZiPqFzR5Fh3oi8td+Se1jaO12vTAouN9jZ28Zh09bWzJAu4/lVjMeTf2/vqzHcOHoSg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-10D</t>
-  </si>
-  <si>
-    <t>Hillside</t>
-  </si>
-  <si>
-    <t>072a216a-7dcf-eb11-8235-002248801d1c</t>
-  </si>
-  <si>
-    <t>YGfaaeMV1tVrfsxOE1q5BtfnxhbEWasc/WhCB0M4w1jE3TLSk6P4XoXsWTdvUPDZizWJAPJRVyb2Kk0KfElrIw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-12D</t>
-  </si>
-  <si>
-    <t>d33523d3-b8bb-eb11-8236-000d3a2aa3e6</t>
-  </si>
-  <si>
-    <t>bwEfzxjV3QTZkAchrI95jB6O9Q72BNimF0Fr+E5Cc9YPQatQWBQgPRflN3HAESXvs1r2CiPlioljzp+e/+1ufA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-14D</t>
-  </si>
-  <si>
-    <t>a25fe136-c8df-eb11-bacb-000d3abc0501</t>
-  </si>
-  <si>
-    <t>nGIyZWpqlykKGjpR1DcwvtnIfK0fW2/z4NyVnLhp3UxTrO2Rhf1glw0u0mlyBjLw6QU7GjD3OU3ARm+zPsJ8ew==</t>
-  </si>
-  <si>
-    <t>OW/HV1-16D</t>
-  </si>
-  <si>
-    <t>410c4583-2b16-ec11-b6e5-6045bd8b892f</t>
-  </si>
-  <si>
-    <t>bC9gaTBL5N5KJ8ZDf3vkDzL+vKXwaEXqxp7MYoXQRH6U9vn7JctbIaYUlgRSbCeFYGqwvSor7UmmdzfKyQXMBw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-17D</t>
-  </si>
-  <si>
-    <t>be7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>tUEZ9xNVG+u3djAGBSsp5oQmW3kM7FYNydt7FHIaL/fVuAXKPKIG/tx/rdeu/oJIN7zQyfZaiDkO91XBn5SA+A==</t>
-  </si>
-  <si>
-    <t>OW/HV1-18A</t>
-  </si>
-  <si>
-    <t>c07a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>7Z8dgiurCfbwR44GB5glOl3Zx89nv95VQ5x+JLMZOgLEdp96ws14d1VdfPNEo0HOKpc9oEmaOHsPg/f/Ee1RgQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-18B</t>
-  </si>
-  <si>
-    <t>c37a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>6hEQvttsYYe+5tITldnplOe4jh79u1LNZ0fEE0sATIz2IHUpocgC87NaMf7jM4KeJlVtRcgdVFRdgA3wFxE3QA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-18C</t>
-  </si>
-  <si>
-    <t>c57a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>W+NwUuro+SZXPOOCdOEZyt7ewtrDh0YKm39vp4VBQlwqgiZ/D2DRot/TqKZ8+b1+bbHCeRzpezdu8CDpAuci/A==</t>
-  </si>
-  <si>
-    <t>OW/HV1-18D</t>
-  </si>
-  <si>
-    <t>Twinhouse</t>
-  </si>
-  <si>
-    <t>6b03c3e7-0a0b-ec11-b6e5-000d3aaf448c</t>
-  </si>
-  <si>
-    <t>HUMlmio1EdCu2Fam+88n/6wFcrEmcO4V93wgoaOr9XmNiCwdFK6iWnQOTpO72zqCWNTWoVxhTDJmZhV+esDMtQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-19B</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>6d03c3e7-0a0b-ec11-b6e5-000d3aaf448c</t>
-  </si>
-  <si>
-    <t>3HXGQ3uAF0SNZ+vUlFTEul4+ptEAuSsR97uC01asaIHLGWlltO3QSBHyhOl9EH5NSVa/Hb1Oq1RZz2hY++qesw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-19C</t>
-  </si>
-  <si>
-    <t>6f03c3e7-0a0b-ec11-b6e5-000d3aaf448c</t>
-  </si>
-  <si>
-    <t>KRqIUWg+i/oe7lrm1xtxd8NE8UitMGLgI+7Vp8BPt77PaPl0F8BboApuBbbrG+6WtxA+IUIDFY0+pP0J1tBxlw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-19D</t>
-  </si>
-  <si>
-    <t>af3523d3-b8bb-eb11-8236-000d3a2aa3e6</t>
-  </si>
-  <si>
-    <t>4Hb9fbTR9JWDiQXSUv6CqwuOUbZ94CsGQT+ITNS5IaKFhooydQZEIRvEeQljTTOqp39w5mldFml3rgTr4okdMA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-1TKB</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>c97a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>7h7rme1qC3TSq3CJ+ReITzjMMOjlY188bXhbHIb2qsu9Tby5f6ykSaz4l5QqOr0uRXkZGPyCZHNs0/OIXzuymw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-20B</t>
-  </si>
-  <si>
-    <t>d37a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>Y+DV810ZXTFsn7H1FxqgKrGTcPZq7fNehHC5OOoEhPmTrMnW5Ilkb9SmDwWuFJ78rYpri9jFICbvE+cE2zdZ8w==</t>
-  </si>
-  <si>
-    <t>OW/HV1-21B</t>
-  </si>
-  <si>
-    <t>d57a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>cbaxaqptmV9e6y3X4B2+DrB44rwQNm4ToL+3cPAB9UV3m0VYxjRMw4cnEvmya8XMqdlzQkPH1iqMpxUyh0nwaA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-21C</t>
-  </si>
-  <si>
-    <t>d77a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>qJqHCx7xzaB2Z3JL5T/lqHAd9W8aH5IvKzT77fQjScedQbLhvyep0yszsMuPimVEvfwDtsPOQ9xFYj84nOBs/w==</t>
-  </si>
-  <si>
-    <t>OW/HV1-21D</t>
-  </si>
-  <si>
-    <t>d97a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>T0xOk3D/cl/0qU4vkHDcGCI3P7owT6GacDrjrlys2fkxHwJR1ktcoxGEKRcqVCdNU8pTQGf54HdaKFhaqo2BXA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-21E</t>
-  </si>
-  <si>
-    <t>ac5fe136-c8df-eb11-bacb-000d3abc0501</t>
-  </si>
-  <si>
-    <t>ZxkPtn6oa9l/0e0uh+z785MlMF/mBZBnz5kZGy0hx4Uxo0BDCshbe8ETCCgPWIH8RaWWTWo2yQHqx7Wyi5ygzQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-22TA</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>de7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>u7IOD+iuQ5sKfDppYLR4h1wbCn7w39a9FYatrkIz5G0ycl41FmZYguHkAyBG+CZiIQRuSaMlI1bejHZfR586Kg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-23B</t>
-  </si>
-  <si>
-    <t>e67a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>cwLcmcvuhFJMO0kTvWeF5SRR0GS2CLSMt0fBLpHEm1WN8VCxpeWej93LjxIdiKnzPDToOUoGmNsFXCzWt0bPEg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-30A</t>
-  </si>
-  <si>
-    <t>eb7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>XiBjgAyX3/P3YUq+5RGRSq2/IcioNNcJfnt0o3/sI4AE9CD3ROYkQfYIiKFSg3l0EANhoYNtQO5XDMjgWe86xQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-30C</t>
-  </si>
-  <si>
-    <t>ef7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>3Waw/y+dN8e1Yq3QYProZOszj1m0XgV3LPZoxs8hanJftSN3/w89oUcsSNqMMjB/tlW/RyqpH94o2jbwn0bpuQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-30E</t>
-  </si>
-  <si>
-    <t>d7a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>SdBQ++rM0MSQlP9FOmMht2dIhTy2rP63P6Hdpz+aW9L0Bh1mt6L1V0QyNZ8b6d1wAef3eOM7mJM2uQ8owBNtWA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-33A</t>
-  </si>
-  <si>
-    <t>d9a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>kApVnIaMjaElQqwBEX5twXnTJeowq+zEt2ZK4CxG1gNSPpp/wgf63TzRxoFRf5UHeTLvmCCkQjRnl/dv99nG3A==</t>
-  </si>
-  <si>
-    <t>OW/HV1-33B</t>
-  </si>
-  <si>
-    <t>dba9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>x5799yTYqlsnPC52b2iyv0Mki0p0GlgSSkyFx+EMQpjuSNB9ct6YHKG3CiNFZqPW+K1dMOM7VYiHxwEEnJLk7g==</t>
-  </si>
-  <si>
-    <t>OW/HV1-33C</t>
-  </si>
-  <si>
-    <t>dda9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>lZnDQ1uD1O33c0I8nshrheSJmblZObhqe4EJkzVXRqgLHnHtCtu7ALRerV1+0O7oUTgsXFNMrRhhhKmZYOJnkw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-33D</t>
-  </si>
-  <si>
-    <t>dfa9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>8PTxyxB2ouNjbHGH1BWXy+bZWF3/jSoseypyt7QABgUVAmopls/cQadhhtVDobmHe/YWSVjs8HTEFdQE9YYOjA==</t>
-  </si>
-  <si>
-    <t>OW/HV1-34A</t>
-  </si>
-  <si>
-    <t>e1a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>hrrtixqGw4gTV9TZX1sdSSZSZazUtgh1b2UDhtBGciZbaaruqQnMoX4spe5SXNc6NRtk0M9K2vmgbLvGFKDXfg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-34B</t>
-  </si>
-  <si>
-    <t>e5a9b009-b03f-ec11-8c60-000d3aae0a5a</t>
-  </si>
-  <si>
-    <t>LmT3c16H7xfuL+B7Wk/g0zXWnVCL9jrwks1+i3qy4draYOZbOr4h5bCnqV5xCHKFuSecL+D+Nebb3w4B7FRqcg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-34D</t>
-  </si>
-  <si>
-    <t>fd7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>GCIpDNkHqX4A8Hss2dfFWFwaiU5qEWfLVu2tNe0GKIHytoreXXqQHrrPuwwtd2YJ+yld3ngcskFASTYhfWbqnQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-35THA</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>ff7a50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>DGnwBSZQO5go6ZRsfoXHMKf/+FaHXiEO4ck7HSkVJXLUzMZVXzQmLAX+qTWJsPOuAFOY25GpQXrCSrH9ehc0YQ==</t>
-  </si>
-  <si>
-    <t>OW/HV1-35THB</t>
-  </si>
-  <si>
-    <t>017b50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>4yY1/rgt8ABrKOoCKUes8fuAgifZDmevoxiCQ7sU4/A+iagCY2reocH56he/OzPmW/yDyjV+eXGZuLtzGt/e8Q==</t>
-  </si>
-  <si>
-    <t>OW/HV1-36A</t>
-  </si>
-  <si>
-    <t>077b50c7-bb26-ec11-b6e5-000d3aa85461</t>
-  </si>
-  <si>
-    <t>yphCM63qZtgqwa6vy1eEhCnYyns6mIJf9WrSbItm1oqHlNwxJSdtqo3VMFGTsE1bE2dqr7USCyTd8iPgyJ+0eg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-36D</t>
-  </si>
-  <si>
-    <t>b838f9db-a6d1-eb11-8235-000d3abe8665</t>
-  </si>
-  <si>
-    <t>u5J4fE6/Z1oBcyUF3CauSQ+hQ61oOmEUz0N632nbvLa0y9j3XRobwH0btpBgOtGk9Lrzajk1Y1Jw3P4A7PQDZg==</t>
-  </si>
-  <si>
-    <t>OW/HV1-43-0-BL</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>ba38f9db-a6d1-eb11-8235-000d3abe8665</t>
-  </si>
-  <si>
-    <t>Vy9uQEYloIRZT+8RFaPaZpdeCyZOgAEKYVEMT7lswXvlDbPWe9+t8dz8fgaEm4yra6sqV84D79ef5K+zYZHtAw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-43-1-BL</t>
-  </si>
-  <si>
-    <t>bc38f9db-a6d1-eb11-8235-000d3abe8665</t>
-  </si>
-  <si>
-    <t>fRj8ikVDxSej1ZM0tezdXeL2rQjs29i4w0Rtq96UFcszVmGoM1D25w/HgCz5UMKMcv+RXCojAld20QIQagJL/w==</t>
-  </si>
-  <si>
-    <t>OW/HV1-43-2-BL</t>
-  </si>
-  <si>
-    <t>c53523d3-b8bb-eb11-8236-000d3a2aa3e6</t>
-  </si>
-  <si>
-    <t>AsyjXTB1xOyTJ2yson9gtfJ9MiFKiITPdsf6eYCD+XLt6Bv3zsBaEDpNv4SwmfLFwV2pGP5s+ySISUwkd7G7hw==</t>
-  </si>
-  <si>
-    <t>OW/HV1-5D</t>
-  </si>
-  <si>
-    <t>2fbceaec-21be-eb11-8236-000d3a2aa437</t>
-  </si>
-  <si>
-    <t>zTXxXfGJg6U7Ue3ELjZcYSbhr3jdiU50OcJg7BOtmB+fH6N9qul0wMmtkeVjO5EP9kOScxk7fhgtjw25qTGs/g==</t>
-  </si>
-  <si>
-    <t>OW/HV1-8D</t>
   </si>
   <si>
     <t>212a216a-7dcf-eb11-8235-002248801d1c</t>
@@ -1739,7 +1739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1774,14 +1774,17 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2121,30 +2124,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="14" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="13" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="13" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="14" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="12" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="15" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="12" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="14" width="14.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -2262,7 +2265,7 @@
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -2313,7 +2316,7 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
@@ -2366,7 +2369,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -2419,7 +2422,7 @@
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -2472,7 +2475,7 @@
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -2527,7 +2530,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -2584,7 +2587,7 @@
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -2641,7 +2644,7 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -2704,7 +2707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>90</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>92</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>4</v>
@@ -2767,21 +2770,21 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C12" s="4">
         <v>44648.5708912037</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>4</v>
@@ -2830,21 +2833,21 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C13" s="4">
         <v>44649.55762731482</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>4</v>
@@ -2891,21 +2894,21 @@
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C14" s="4">
         <v>44648.645520833335</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>4</v>
@@ -2954,21 +2957,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="C15" s="4">
         <v>44714.461851851855</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>4</v>
@@ -3019,21 +3022,21 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C16" s="4">
         <v>44692.4047337963</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -3080,21 +3083,21 @@
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="C17" s="4">
         <v>44692.404699074075</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>88</v>
@@ -3143,21 +3146,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="C18" s="4">
         <v>44692.40472222222</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>88</v>
@@ -3204,27 +3207,27 @@
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C19" s="4">
         <v>44692.404699074075</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>26</v>
@@ -3265,21 +3268,21 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="C20" s="4">
         <v>44649.42019675926</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>88</v>
@@ -3315,7 +3318,7 @@
         <v>83</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R20" s="8">
         <v>3</v>
@@ -3328,21 +3331,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C21" s="4">
         <v>44649.423113425924</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>88</v>
@@ -3378,7 +3381,7 @@
         <v>83</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R21" s="8">
         <v>3</v>
@@ -3391,21 +3394,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C22" s="4">
         <v>44649.42072916667</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>88</v>
@@ -3441,7 +3444,7 @@
         <v>83</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R22" s="8">
         <v>3</v>
@@ -3454,27 +3457,27 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C23" s="4">
         <v>44648.5708912037</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>26</v>
@@ -3504,7 +3507,7 @@
         <v>143</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R23" s="8">
         <v>3</v>
@@ -3515,21 +3518,21 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C24" s="4">
         <v>44697.575787037036</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>88</v>
@@ -3565,7 +3568,7 @@
         <v>83</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R24" s="8">
         <v>3</v>
@@ -3578,21 +3581,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C25" s="4">
         <v>44692.40472222222</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>88</v>
@@ -3628,7 +3631,7 @@
         <v>83</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R25" s="8">
         <v>3</v>
@@ -3639,21 +3642,21 @@
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C26" s="4">
         <v>44692.404756944445</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>88</v>
@@ -3689,7 +3692,7 @@
         <v>83</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R26" s="8">
         <v>3</v>
@@ -3702,21 +3705,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="C27" s="4">
         <v>44692.4047337963</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>88</v>
@@ -3752,7 +3755,7 @@
         <v>83</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R27" s="8">
         <v>3</v>
@@ -3763,21 +3766,21 @@
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="C28" s="4">
         <v>44692.4047337963</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>4</v>
@@ -3813,7 +3816,7 @@
         <v>85</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R28" s="8">
         <v>3</v>
@@ -3824,27 +3827,27 @@
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="C29" s="4">
         <v>44648.5708912037</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>26</v>
@@ -3874,7 +3877,7 @@
         <v>135</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R29" s="8">
         <v>4</v>
@@ -3885,21 +3888,21 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="C30" s="4">
         <v>44648.645532407405</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>88</v>
@@ -3935,7 +3938,7 @@
         <v>83</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R30" s="8">
         <v>3</v>
@@ -3948,21 +3951,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="C31" s="4">
         <v>44649.55762731482</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>4</v>
@@ -3998,7 +4001,7 @@
         <v>85</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R31" s="8">
         <v>3</v>
@@ -4009,21 +4012,21 @@
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="C32" s="4">
         <v>44649.55762731482</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>88</v>
@@ -4059,7 +4062,7 @@
         <v>83</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R32" s="8">
         <v>3</v>
@@ -4070,21 +4073,21 @@
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="C33" s="4">
         <v>44649.55763888889</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>4</v>
@@ -4120,7 +4123,7 @@
         <v>85</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R33" s="8">
         <v>3</v>
@@ -4131,21 +4134,21 @@
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="C34" s="4">
         <v>44692.4047337963</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>4</v>
@@ -4194,21 +4197,21 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="C35" s="4">
         <v>44694.63408564815</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>88</v>
@@ -4259,19 +4262,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C36" s="4">
         <v>44694.63418981482</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>88</v>
@@ -4322,19 +4325,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="C37" s="4">
         <v>44692.404756944445</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>4</v>
@@ -4385,19 +4388,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="C38" s="4">
         <v>44692.404756944445</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>4</v>
@@ -4448,19 +4451,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C39" s="4">
         <v>44704.499375</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>88</v>
@@ -4511,19 +4514,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="C40" s="4">
         <v>44692.404756944445</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>4</v>
@@ -4574,19 +4577,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="C41" s="4">
         <v>44708.411087962966</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -4622,7 +4625,7 @@
         <v>115</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R41" s="8">
         <v>4</v>
@@ -4635,19 +4638,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="15.75">
       <c r="A42" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C42" s="4">
         <v>44708.41116898148</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>1</v>
@@ -4683,7 +4686,7 @@
         <v>115</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R42" s="8">
         <v>4</v>
@@ -4696,19 +4699,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="15.75">
       <c r="A43" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="C43" s="4">
         <v>44649.55763888889</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>4</v>
@@ -4757,19 +4760,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="15.75">
       <c r="A44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="C44" s="4">
         <v>44649.55763888889</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -4818,19 +4821,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="15.75">
       <c r="A45" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C45" s="4">
         <v>44648.570914351854</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>8</v>
@@ -4866,7 +4869,7 @@
         <v>70</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R45" s="8">
         <v>3</v>
@@ -4879,19 +4882,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="15.75">
       <c r="A46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="C46" s="4">
         <v>44648.570925925924</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>8</v>
@@ -4925,7 +4928,7 @@
         <v>70</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R46" s="8">
         <v>3</v>
@@ -4938,19 +4941,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="15.75">
       <c r="A47" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="C47" s="4">
         <v>44648.570925925924</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>8</v>
@@ -4984,7 +4987,7 @@
         <v>67</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R47" s="8">
         <v>3</v>
@@ -4997,19 +5000,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="15.75">
       <c r="A48" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="C48" s="4">
         <v>44648.57094907408</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>4</v>
@@ -5060,19 +5063,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="15.75">
       <c r="A49" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="C49" s="4">
         <v>44648.57098379629</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>4</v>
@@ -5135,7 +5138,7 @@
         <v>216</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>4</v>
@@ -5198,7 +5201,7 @@
         <v>219</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>88</v>
@@ -5261,7 +5264,7 @@
         <v>222</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>88</v>
@@ -5324,7 +5327,7 @@
         <v>225</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>4</v>
@@ -5387,13 +5390,13 @@
         <v>228</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>26</v>
@@ -5450,7 +5453,7 @@
         <v>231</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>88</v>
@@ -5513,7 +5516,7 @@
         <v>234</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>4</v>
@@ -5576,7 +5579,7 @@
         <v>237</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>4</v>
@@ -5612,7 +5615,7 @@
         <v>85</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R57" s="8">
         <v>3</v>
@@ -5639,7 +5642,7 @@
         <v>240</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>4</v>
@@ -5675,7 +5678,7 @@
         <v>85</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R58" s="8">
         <v>3</v>
@@ -5702,7 +5705,7 @@
         <v>243</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>4</v>
@@ -5738,7 +5741,7 @@
         <v>85</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R59" s="8">
         <v>3</v>
@@ -5765,7 +5768,7 @@
         <v>246</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>4</v>
@@ -5801,7 +5804,7 @@
         <v>85</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R60" s="8">
         <v>3</v>
@@ -5828,7 +5831,7 @@
         <v>249</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>6</v>
@@ -5889,7 +5892,7 @@
         <v>254</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>6</v>
@@ -5950,7 +5953,7 @@
         <v>257</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>4</v>
@@ -6013,7 +6016,7 @@
         <v>260</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>6</v>

</xml_diff>